<commit_message>
upload goc , actual , chart
</commit_message>
<xml_diff>
--- a/WISOL.UI/Worksheet_PR.xlsx
+++ b/WISOL.UI/Worksheet_PR.xlsx
@@ -12,13 +12,13 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
-    <sheet name="3rd" sheetId="2" r:id="rId1"/>
+    <sheet name="Order" sheetId="2" r:id="rId1"/>
     <sheet name="Char" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'3rd'!$A$1:$U$76</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Char!$A$1:$S$77</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'3rd'!$10:$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Order!$A$1:$U$76</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Order!$10:$12</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -38,9 +38,6 @@
     <t>BỘ PHẬN: SMT</t>
   </si>
   <si>
-    <t>1. 구입 목적 (Mục đích mua) : 20년 9 월 생산계획에 따른 Consumable part 구입 품의 (Đề nghị mua vật tư tiêu hao dựa trên kế hoạch sản xuất tháng 9 năm 2020)</t>
-  </si>
-  <si>
     <t>2.Lead Time : P/O Open 후 30 day (30 ngày sau ngày P/O)</t>
   </si>
   <si>
@@ -57,30 +54,6 @@
   </si>
   <si>
     <t>Tên vật tư tiếng Việt</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <rFont val="바탕"/>
-        <family val="1"/>
-        <charset val="129"/>
-      </rPr>
-      <t xml:space="preserve">
-Tên t</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>iếng anh/ tiếng hàn</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Quy cách /
@@ -292,6 +265,54 @@
   </si>
   <si>
     <t>4.구매 요청(PR.NO):</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="바탕"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Tên</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="바탕"/>
+        <family val="1"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>tiếng anh/ tiếng hàn</t>
+    </r>
+  </si>
+  <si>
+    <t>1. 구입 목적 (Mục đích mua) : ….년 ... 월 생산계획에 따른 Consumable part 구입 품의 (Đề nghị mua vật tư tiêu hao dựa trên kế hoạch sản xuất tháng …. năm ….)</t>
   </si>
 </sst>
 </file>
@@ -673,7 +694,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -820,6 +841,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1185,7 +1209,7 @@
   <dimension ref="A2:U59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="57" zoomScalePageLayoutView="69" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:T3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
@@ -1207,102 +1231,102 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="43.9" customHeight="1">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58"/>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="58"/>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
     </row>
     <row r="3" spans="1:21" s="1" customFormat="1" ht="43.9" customHeight="1">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="58"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
     </row>
     <row r="4" spans="1:21" ht="28.9" customHeight="1">
-      <c r="A4" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59"/>
-      <c r="T4" s="59"/>
+      <c r="A4" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="60"/>
+      <c r="T4" s="60"/>
     </row>
     <row r="5" spans="1:21" ht="42" customHeight="1"/>
     <row r="6" spans="1:21" s="6" customFormat="1" ht="42" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:21" s="6" customFormat="1" ht="42" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:21" s="6" customFormat="1" ht="42" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:21" s="12" customFormat="1" ht="32.450000000000003" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1325,155 +1349,155 @@
       <c r="T9" s="8"/>
     </row>
     <row r="10" spans="1:21" s="13" customFormat="1" ht="40.9" customHeight="1">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="L10" s="57"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
+      <c r="O10" s="57"/>
+      <c r="P10" s="57"/>
+      <c r="Q10" s="57"/>
+      <c r="R10" s="57"/>
+      <c r="S10" s="57"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="58"/>
+    </row>
+    <row r="11" spans="1:21" s="13" customFormat="1" ht="94.9" customHeight="1">
+      <c r="A11" s="61"/>
+      <c r="B11" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="56"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="56"/>
-      <c r="Q10" s="56"/>
-      <c r="R10" s="56"/>
-      <c r="S10" s="56"/>
-      <c r="T10" s="56"/>
-      <c r="U10" s="57"/>
-    </row>
-    <row r="11" spans="1:21" s="13" customFormat="1" ht="94.9" customHeight="1">
-      <c r="A11" s="60"/>
-      <c r="B11" s="60" t="s">
+      <c r="C11" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="D11" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="E11" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="G11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="H11" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="I11" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="J11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="K11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="15" t="s">
+      <c r="L11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="M11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="N11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="O11" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="N11" s="16" t="s">
+      <c r="P11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="O11" s="14" t="s">
+      <c r="Q11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="P11" s="14" t="s">
+      <c r="R11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="Q11" s="14" t="s">
+      <c r="S11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="R11" s="14" t="s">
+      <c r="T11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="S11" s="14" t="s">
+      <c r="U11" s="51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="13" customFormat="1" ht="71.45" customHeight="1">
+      <c r="A12" s="61"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="T11" s="14" t="s">
+      <c r="F12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="U11" s="51" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="13" customFormat="1" ht="71.45" customHeight="1">
-      <c r="A12" s="60"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="14" t="s">
+      <c r="G12" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="H12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="I12" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="J12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="K12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="L12" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="17" t="s">
+      <c r="M12" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="L12" s="17" t="s">
+      <c r="N12" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="17" t="s">
+      <c r="O12" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="N12" s="14" t="s">
+      <c r="P12" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="O12" s="14" t="s">
+      <c r="Q12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="P12" s="14" t="s">
+      <c r="R12" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="Q12" s="14" t="s">
+      <c r="S12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="R12" s="14" t="s">
+      <c r="T12" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="S12" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="T12" s="14" t="s">
-        <v>40</v>
-      </c>
       <c r="U12" s="51" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="30" customFormat="1" ht="187.5" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="20"/>
@@ -1786,7 +1810,7 @@
   <sheetData>
     <row r="1" spans="2:18">
       <c r="B1" s="39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G1" s="40"/>
     </row>

</xml_diff>